<commit_message>
updated excel taxable and total dividends.
</commit_message>
<xml_diff>
--- a/DividendLiberty/bin/Debug/Dividend Calculation.xlsx
+++ b/DividendLiberty/bin/Debug/Dividend Calculation.xlsx
@@ -582,7 +582,7 @@
   <dimension ref="B1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,7 +788,7 @@
         <v>8</v>
       </c>
       <c r="L6" s="9">
-        <v>8.34</v>
+        <v>44.12</v>
       </c>
       <c r="M6" s="10">
         <v>7.76</v>
@@ -798,7 +798,7 @@
       </c>
       <c r="O6" s="12">
         <f t="shared" si="1"/>
-        <v>30.910000000000004</v>
+        <v>66.69</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
@@ -1146,7 +1146,7 @@
       </c>
       <c r="L15" s="3">
         <f>SUM(L3:L14)</f>
-        <v>293.75999999999993</v>
+        <v>329.53999999999996</v>
       </c>
       <c r="M15" s="4">
         <f>SUM(M3:M14)</f>
@@ -1158,7 +1158,7 @@
       </c>
       <c r="O15" s="6">
         <f>SUM(O3:O14)</f>
-        <v>465.8</v>
+        <v>501.58</v>
       </c>
     </row>
   </sheetData>
@@ -1171,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="F8" s="9">
         <f>Yearly!L15</f>
-        <v>293.75999999999993</v>
+        <v>329.53999999999996</v>
       </c>
       <c r="G8" s="10">
         <f>Yearly!M15</f>
@@ -1274,7 +1274,7 @@
       </c>
       <c r="I8" s="12">
         <f t="shared" si="0"/>
-        <v>465.79999999999995</v>
+        <v>501.58</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -2061,7 +2061,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="3">
         <f>SUM(F6:F45)</f>
-        <v>1321.6599999999999</v>
+        <v>1357.4399999999998</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" ref="G46:I46" si="1">SUM(G6:G45)</f>
@@ -2073,7 +2073,7 @@
       </c>
       <c r="I46" s="6">
         <f t="shared" si="1"/>
-        <v>1821.27</v>
+        <v>1857.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated taxable dividend and all dividend excel files.
</commit_message>
<xml_diff>
--- a/DividendLiberty/bin/Debug/Dividend Calculation.xlsx
+++ b/DividendLiberty/bin/Debug/Dividend Calculation.xlsx
@@ -548,7 +548,7 @@
   <dimension ref="B1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,7 +834,7 @@
         <v>10</v>
       </c>
       <c r="L8" s="9">
-        <v>142.19999999999999</v>
+        <v>152.4</v>
       </c>
       <c r="M8" s="10">
         <v>51.06</v>
@@ -844,7 +844,7 @@
       </c>
       <c r="O8" s="12">
         <f t="shared" si="1"/>
-        <v>235.57</v>
+        <v>245.77</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
@@ -1112,7 +1112,7 @@
       </c>
       <c r="L15" s="3">
         <f>SUM(L3:L14)</f>
-        <v>610.71</v>
+        <v>620.91</v>
       </c>
       <c r="M15" s="4">
         <f>SUM(M3:M14)</f>
@@ -1124,7 +1124,7 @@
       </c>
       <c r="O15" s="6">
         <f>SUM(O3:O14)</f>
-        <v>935.29</v>
+        <v>945.49</v>
       </c>
     </row>
   </sheetData>
@@ -1137,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="F8" s="9">
         <f>Yearly!L15</f>
-        <v>610.71</v>
+        <v>620.91</v>
       </c>
       <c r="G8" s="10">
         <f>Yearly!M15</f>
@@ -1240,7 +1240,7 @@
       </c>
       <c r="I8" s="12">
         <f t="shared" si="0"/>
-        <v>935.29000000000008</v>
+        <v>945.49</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -2027,7 +2027,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="3">
         <f>SUM(F6:F45)</f>
-        <v>1638.61</v>
+        <v>1648.81</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" ref="G46:I46" si="1">SUM(G6:G45)</f>
@@ -2039,7 +2039,7 @@
       </c>
       <c r="I46" s="6">
         <f t="shared" si="1"/>
-        <v>2290.7600000000002</v>
+        <v>2300.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>